<commit_message>
Aggiunto caso di test 25 (fast track)
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#ADLINGEGNERIAINFORMATICAXX/ADL/ARIA/2.99.2/report-checklis.xlsx
+++ b/GATEWAY/A1#111#ADLINGEGNERIAINFORMATICAXX/ADL/ARIA/2.99.2/report-checklis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utente\Desktop\Nuovo accreditamento\PSS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utente\Desktop\ARIA\_PSS\it-fse-accreditamento\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{937FBF9C-FE70-468F-A2B2-73BFCE2FCF09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4447D50-BD74-4D9C-8CC6-F19584E51A89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="421" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="421" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="240">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -995,6 +995,22 @@
   </si>
   <si>
     <t>ADL</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_PSS_CT25</t>
+  </si>
+  <si>
+    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation", al fine di una futura pubblicazione, con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+Il Documento CDA2 Profilo Sanitario Sintetico dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. Il "CASO DI TEST 25" si riferisce a un esempio di CDA2 semplice, contenente esclusivamente sezioni ed elementi obbligatori previsti dalle specifiche nazionali (IG HL7 Italia)</t>
+  </si>
+  <si>
+    <t>2025-12-05T16:35:54Z</t>
+  </si>
+  <si>
+    <t>e2768f51eb906092f8e4edd87a20072d</t>
+  </si>
+  <si>
+    <t>6506aa66-1c27-4e22-abcc-e215717942f0.9c717939a2a9a31bd0fab64231e9b14ca6e2d16958b3a06f57f0701c867c9b72.8063141458^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -1137,7 +1153,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -1472,12 +1488,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1626,6 +1657,30 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3103,11 +3158,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:W619"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B27" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" ySplit="9" topLeftCell="B30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="B31" sqref="B31"/>
+      <selection pane="bottomRight" activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4705,25 +4760,52 @@
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="F32" s="12"/>
-      <c r="G32" s="12"/>
-      <c r="H32" s="12"/>
-      <c r="I32" s="12"/>
-      <c r="J32" s="13"/>
-      <c r="K32" s="13"/>
-      <c r="L32" s="13"/>
-      <c r="M32" s="13"/>
-      <c r="N32" s="13"/>
-      <c r="O32" s="13"/>
-      <c r="P32" s="13"/>
-      <c r="Q32" s="13"/>
-      <c r="R32" s="13"/>
-      <c r="S32" s="13"/>
-      <c r="T32" s="13"/>
-      <c r="U32" s="14"/>
-      <c r="V32" s="2"/>
-      <c r="W32" s="15"/>
+    <row r="32" spans="1:23" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="59">
+        <v>478</v>
+      </c>
+      <c r="B32" s="59" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" s="60" t="s">
+        <v>48</v>
+      </c>
+      <c r="D32" s="59" t="s">
+        <v>235</v>
+      </c>
+      <c r="E32" s="61" t="s">
+        <v>236</v>
+      </c>
+      <c r="F32" s="62">
+        <v>45996</v>
+      </c>
+      <c r="G32" s="62" t="s">
+        <v>237</v>
+      </c>
+      <c r="H32" s="62" t="s">
+        <v>238</v>
+      </c>
+      <c r="I32" s="63" t="s">
+        <v>239</v>
+      </c>
+      <c r="J32" s="64" t="s">
+        <v>53</v>
+      </c>
+      <c r="K32" s="64"/>
+      <c r="L32" s="64"/>
+      <c r="M32" s="64"/>
+      <c r="N32" s="64"/>
+      <c r="O32" s="64"/>
+      <c r="P32" s="64"/>
+      <c r="Q32" s="64"/>
+      <c r="R32" s="64"/>
+      <c r="S32" s="64"/>
+      <c r="T32" s="64"/>
+      <c r="U32" s="65"/>
+      <c r="V32" s="66"/>
+      <c r="W32" s="64" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="33" spans="6:23" x14ac:dyDescent="0.25">
       <c r="F33" s="12"/>
@@ -12203,6 +12285,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">137048 - Stesura checklist RAP</UserStoryALM>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="18" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="152ec67562f6729267530f2154e17cab">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bea1cbc65ad49ac624eb199c90a8cd28" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -12460,28 +12563,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">137048 - Stesura checklist RAP</UserStoryALM>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C0F090B6-07CB-41CE-9867-FFD42C97BE05}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12498,29 +12605,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>